<commit_message>
Updated tubing and valves
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Documents\GitHub\Operant_Temp_Assay_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8BB84A-E137-4122-BD9F-405E4D631331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32095131-B7A8-4DAD-8FF3-439D398EA2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="18264" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>Masterflex L/S® Precision Pump Tubing, Platinum-Cured Silicone, L/S 16; 25 ft</t>
   </si>
@@ -114,15 +114,9 @@
     <t>https://www.adafruit.com/product/1480</t>
   </si>
   <si>
-    <t>2.2" 18-bit color TFT LCD display with microSD card breakout</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/2590</t>
   </si>
   <si>
-    <t>Adafruit Metro Mini 328 - Arduino-Compatible - 5V 16MHz</t>
-  </si>
-  <si>
     <t>Adafruit Universal Thermocouple Amplifier MAX31856 Breakout</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t xml:space="preserve">Total </t>
   </si>
   <si>
-    <t>Tubing</t>
-  </si>
-  <si>
     <t>Electronics</t>
   </si>
   <si>
@@ -180,18 +171,6 @@
     <t>USB Mini Hub with Power Switch</t>
   </si>
   <si>
-    <t>https://www.sciplus.com/12-vdc-solenoid-valve-10pack-savings-54414-p</t>
-  </si>
-  <si>
-    <t>12 VDC SOLENOID VALVE 10-PACK SAVINGS</t>
-  </si>
-  <si>
-    <t>40672P10</t>
-  </si>
-  <si>
-    <t>Sciplus</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/368</t>
   </si>
   <si>
@@ -252,27 +231,12 @@
     <t>Refrigeration Tubing Copper Tubing Coil 3mm OD x 2mm ID x 24.5Ft Length - Walmart.com - Walmart.com</t>
   </si>
   <si>
-    <t>Refrigeration Tubing Copper Tubing Coil 3mm OD 2mm ID 16Ft Length</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Electric-Solenoid-Automatic-Drinking-Fountains-no/dp/B0BP7KC8VJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/8inch 12VDC Hose Barb Electric Solenoid Valve Plastic Body 12-Volt DC for Automatic Faucets Drinking Fountains-no Pressure,White &amp; Black </t>
-  </si>
-  <si>
     <t>qty: 2+spare</t>
   </si>
   <si>
     <t>https://www.amazon.com/SNS-2WK025-N08-Electric-Solenoid-Normally/dp/B07SPK59LP/</t>
   </si>
   <si>
-    <t>2WK025-N08</t>
-  </si>
-  <si>
-    <t>DC12V 1/4" NPT Electric Solenoid Valve Normally Open</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/5233K958/</t>
   </si>
   <si>
@@ -318,31 +282,79 @@
     <t>https://www.mcmaster.com/5233K56/</t>
   </si>
   <si>
-    <t>1/4" ID tubing</t>
-  </si>
-  <si>
     <t>5233K56</t>
   </si>
   <si>
     <t>91355K31</t>
   </si>
   <si>
-    <t>1/4" to 1/8" hose barb adapter</t>
-  </si>
-  <si>
-    <t>8 mm to 6 mm (~1/4") hose barb adapter</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/5218K434/</t>
   </si>
   <si>
     <t>5218K434</t>
   </si>
   <si>
-    <t>1/8" hose barb Tee connector connec</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Brass-Splicer-Union-Fitting-123-2/dp/B07GQPF7FS?th=1</t>
+    <t>qty: 4+spare</t>
+  </si>
+  <si>
+    <t>1/8" hose barb Tee connector</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91355K57/</t>
+  </si>
+  <si>
+    <t>91355K57</t>
+  </si>
+  <si>
+    <t>1/4" to 1/8" hose barb adapter (for reducer)</t>
+  </si>
+  <si>
+    <t>1/4" ID tubing (for reducer)</t>
+  </si>
+  <si>
+    <t>8 mm to 6 mm (~1/4") hose barb adapter (for reducer)</t>
+  </si>
+  <si>
+    <t>qty: pack of 5 (2+3 spare)</t>
+  </si>
+  <si>
+    <t>qty: 2 packs of 2 (2+2 spare)</t>
+  </si>
+  <si>
+    <t>12VDC 1/4" NPT Electric Solenoid Valve Normally Open (large valves)</t>
+  </si>
+  <si>
+    <t>qty: 6+2 spare</t>
+  </si>
+  <si>
+    <t>Tubing and valves</t>
+  </si>
+  <si>
+    <t>1/8" NPT to 1/8" ID hose barb adapter</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/5463K438/</t>
+  </si>
+  <si>
+    <t>5463K438</t>
+  </si>
+  <si>
+    <t>qty: pack of 10 (8+2 spare)</t>
+  </si>
+  <si>
+    <t>12VDC 1/8" NPT Electric Solenoid Valve Normally Closed (small valves)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Brass-Electric-Solenoid-Normally-Closed/dp/B01M5IXT4D/</t>
+  </si>
+  <si>
+    <t>Copper Tubing, 3mm OD, 2mm ID, 16 ft Length</t>
+  </si>
+  <si>
+    <t>(optional display) 2.2" 18-bit color TFT LCD display with microSD card breakout</t>
+  </si>
+  <si>
+    <t>(optional display controller) Adafruit Metro Mini 328 - Arduino-Compatible - 5V 16MHz</t>
   </si>
 </sst>
 </file>
@@ -424,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -453,14 +465,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -468,17 +474,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -764,8 +791,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,14 +805,14 @@
     <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -806,24 +833,24 @@
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>36</v>
+      <c r="A2" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>89</v>
+      <c r="C2" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -836,313 +863,327 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>17.32</v>
+      </c>
+      <c r="H3" s="2">
+        <f>G3*F3</f>
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>91.5</v>
+      </c>
+      <c r="H4" s="2">
+        <f>G4*F4</f>
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>19.559999999999999</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.42</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>13.26</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>13.26</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8" si="1">G8*F8</f>
+        <v>1.7399999999999998</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="19">
+        <v>8</v>
+      </c>
+      <c r="G10" s="20">
+        <v>4.62</v>
+      </c>
+      <c r="H10" s="20">
+        <f t="shared" si="0"/>
+        <v>36.96</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="19">
+        <v>1</v>
+      </c>
+      <c r="G11" s="20">
+        <v>14.08</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" ref="H11" si="2">G11*F11</f>
+        <v>14.08</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>24.99</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" si="0"/>
-        <v>24.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>17.32</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>17.32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F12" s="19">
         <v>3</v>
       </c>
-      <c r="G5" s="2">
-        <v>2.42</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>7.26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>13.26</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>13.26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" ref="H7" si="1">G7*F7</f>
-        <v>1.7399999999999998</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>91.5</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>91.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="1">
-        <v>4</v>
-      </c>
-      <c r="G10" s="2">
-        <v>4.62</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>18.48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4">
-        <v>3</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="G12" s="20">
         <v>20.99</v>
       </c>
-      <c r="H11" s="5">
-        <f t="shared" si="0"/>
+      <c r="H12" s="20">
+        <f>G12*F12</f>
         <v>62.97</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>11.99</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>11.99</v>
+      <c r="I12" s="19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="B13" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="4">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5">
         <v>7.86</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>23.580000000000002</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="H13" s="5">
+        <f>G13*F13</f>
+        <v>39.300000000000004</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>9</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>9.9499999999999993</v>
+        <v>11.99</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>9.9499999999999993</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1166,11 +1207,11 @@
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1194,19 +1235,19 @@
         <v>6</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1223,15 +1264,15 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1248,15 +1289,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
@@ -1273,7 +1314,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1298,12 +1339,12 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
         <v>196</v>
@@ -1322,12 +1363,12 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="1">
@@ -1347,13 +1388,13 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1">
         <v>2590</v>
@@ -1373,12 +1414,12 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D24" s="1">
         <v>3263</v>
@@ -1398,12 +1439,12 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1">
         <v>270</v>
@@ -1422,16 +1463,16 @@
         <v>19.899999999999999</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1">
         <v>826</v>
@@ -1451,12 +1492,12 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1">
         <v>352</v>
@@ -1476,12 +1517,12 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D28" s="1">
         <v>368</v>
@@ -1501,12 +1542,12 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1">
         <v>592</v>
@@ -1526,12 +1567,12 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4">
         <v>2998</v>
@@ -1551,8 +1592,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
-        <v>42</v>
+      <c r="A31" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>18</v>
@@ -1578,18 +1619,18 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1602,37 +1643,38 @@
         <v>50</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G33" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H33" s="2">
         <f>SUM(H2:H32)</f>
-        <v>675.9</v>
+        <v>713.6400000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A12:A30"/>
-    <mergeCell ref="A2:A11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{D129A47F-42A4-439A-9FB8-0EB478ADE2C4}"/>
     <hyperlink ref="C16" r:id="rId2" xr:uid="{1CA04464-0DE8-4D1E-8969-86ABEF326FAC}"/>
-    <hyperlink ref="C12" r:id="rId3" xr:uid="{1999E1EB-570D-4500-8C89-5F00B4DEFDBF}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{1999E1EB-570D-4500-8C89-5F00B4DEFDBF}"/>
     <hyperlink ref="C31" r:id="rId4" xr:uid="{E56B4AF8-2872-45E8-9B43-F249B28D2B25}"/>
     <hyperlink ref="C23" r:id="rId5" xr:uid="{DCFAFB62-316E-4588-8E59-7CB94BD04D81}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{6FDB28B5-CEF2-40E0-983E-538007902B6E}"/>
-    <hyperlink ref="C17" r:id="rId7" xr:uid="{B709335A-C16D-400A-BF0D-CE31E5535D6F}"/>
-    <hyperlink ref="C19" r:id="rId8" xr:uid="{48B1CEBC-8B82-444F-9BB0-639FE74A5145}"/>
-    <hyperlink ref="C4" r:id="rId9" display="https://www.walmart.com/ip/Refrigeration-Tubing-Copper-Tubing-Coil-3mm-OD-x-2mm-ID-x-24-5Ft-Length/426649156?wmlspartner=wmtlabs&amp;adid=22222222222392976812&amp;wmlspartner=wmtlabs&amp;wl0=e&amp;wl1=o&amp;wl2=c&amp;wl3=74492048069633&amp;wl4=pla-4578091583802856&amp;wl5=&amp;wl6=&amp;wl7=&amp;wl10=Walmart&amp;wl11=Online&amp;wl12=426649156_10000000599&amp;wl14=refrigeration%20copper%20tubing%203%20mm&amp;veh=sem&amp;gclid=5f207a189dae1cb7dd391a839d73171a&amp;gclsrc=3p.ds&amp;msclkid=5f207a189dae1cb7dd391a839d73171a" xr:uid="{CB83F98A-B10F-49B4-9ABF-1C89C99A8A17}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{434F19D0-7432-495C-9FDE-4F93DA984FD2}"/>
+    <hyperlink ref="C17" r:id="rId6" xr:uid="{B709335A-C16D-400A-BF0D-CE31E5535D6F}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{48B1CEBC-8B82-444F-9BB0-639FE74A5145}"/>
+    <hyperlink ref="C3" r:id="rId8" display="https://www.walmart.com/ip/Refrigeration-Tubing-Copper-Tubing-Coil-3mm-OD-x-2mm-ID-x-24-5Ft-Length/426649156?wmlspartner=wmtlabs&amp;adid=22222222222392976812&amp;wmlspartner=wmtlabs&amp;wl0=e&amp;wl1=o&amp;wl2=c&amp;wl3=74492048069633&amp;wl4=pla-4578091583802856&amp;wl5=&amp;wl6=&amp;wl7=&amp;wl10=Walmart&amp;wl11=Online&amp;wl12=426649156_10000000599&amp;wl14=refrigeration%20copper%20tubing%203%20mm&amp;veh=sem&amp;gclid=5f207a189dae1cb7dd391a839d73171a&amp;gclsrc=3p.ds&amp;msclkid=5f207a189dae1cb7dd391a839d73171a" xr:uid="{CB83F98A-B10F-49B4-9ABF-1C89C99A8A17}"/>
+    <hyperlink ref="C4" r:id="rId9" xr:uid="{434F19D0-7432-495C-9FDE-4F93DA984FD2}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{80616FD6-BA5D-46E8-9D99-F241EC20E680}"/>
+    <hyperlink ref="C24" r:id="rId11" xr:uid="{47454E5A-1F66-48D4-91F9-4EC9944817E5}"/>
+    <hyperlink ref="C10" r:id="rId12" xr:uid="{D1A2362F-1EC5-4F17-8C38-DA3C2CBCA9AC}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{77F69606-E9D6-42F3-9CBF-86F64ECD0272}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>